<commit_message>
add some files such as openpyxl_offset.ipoynb
</commit_message>
<xml_diff>
--- a/Chapter-12-4-1.xlsx
+++ b/Chapter-12-4-1.xlsx
@@ -1,75 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\Chapter-12\Chapter-12-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repos\fish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F23BC0-62CC-4DD9-9C8D-9E68B4645733}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A08FB90F-F7C0-4918-A184-BEDF65BB65EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8475" yWindow="3855" windowWidth="22065" windowHeight="7110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11232" yWindow="0" windowWidth="11544" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="分数表" sheetId="1" r:id="rId1"/>
+    <sheet name="xlwings转换后" sheetId="3" r:id="rId1"/>
+    <sheet name="分数表" sheetId="1" r:id="rId2"/>
+    <sheet name="转换后" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+  <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>科目</t>
+  </si>
+  <si>
+    <t>分数</t>
+  </si>
   <si>
     <t>小张</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语文</t>
+  </si>
+  <si>
+    <t>数学</t>
+  </si>
+  <si>
+    <t>英语</t>
   </si>
   <si>
     <t>李飞</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>英语</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>科目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小曾</t>
   </si>
   <si>
     <t>小江</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小曾</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -415,29 +397,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B605C6-DF67-49B1-BBE4-5BCEF9E388A4}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>96</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+      <c r="C4">
+        <v>99</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>95</v>
+      </c>
+      <c r="D5">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -446,9 +504,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -457,9 +515,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -468,9 +526,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -479,9 +537,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -490,9 +548,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -501,9 +559,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -512,9 +570,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -523,9 +581,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -537,6 +595,81 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>96</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+      <c r="C4">
+        <v>99</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>95</v>
+      </c>
+      <c r="D5">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>